<commit_message>
Split to two Modules
</commit_message>
<xml_diff>
--- a/Liste der APIs.xlsx
+++ b/Liste der APIs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\BlizzAPIs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2A2201-CA35-4941-8379-7DB8027E829B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41BFE76-ACF0-4E28-87E7-70488F164119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{45ECA79C-1FAA-4BE6-AC11-91FC7F2CF522}"/>
+    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="15840" xr2:uid="{45ECA79C-1FAA-4BE6-AC11-91FC7F2CF522}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data APIs" sheetId="2" r:id="rId1"/>
@@ -746,7 +746,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,6 +798,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -859,7 +873,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -892,6 +906,12 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
@@ -1285,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FB894B-C5F2-4F1D-A33C-BFF7078F46A6}">
   <dimension ref="A1:I961"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,16 +1327,16 @@
       <c r="A1" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -4604,8 +4624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF5CD30-F5AE-4240-A3D1-394B1D8EAD48}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed Verb from Request to Get
</commit_message>
<xml_diff>
--- a/Liste der APIs.xlsx
+++ b/Liste der APIs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\BlizzAPIs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37847436-3B7A-4A17-A926-32E78EF3F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54AE3CD-5C27-4B26-9A75-7FDC303A50CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="285" windowWidth="29040" windowHeight="15840" xr2:uid="{45ECA79C-1FAA-4BE6-AC11-91FC7F2CF522}"/>
   </bookViews>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:I961"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1673,7 @@
       <c r="D23" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>92</v>
       </c>
       <c r="F23" s="9" t="s">
@@ -4590,7 +4590,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>